<commit_message>
baby charts are back!
</commit_message>
<xml_diff>
--- a/flights-data/usa_out.xlsx
+++ b/flights-data/usa_out.xlsx
@@ -1,37 +1,177 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+  <si>
+    <t>date_</t>
+  </si>
+  <si>
+    <t>scheduled_mean</t>
+  </si>
+  <si>
+    <t>scheduled_sum</t>
+  </si>
+  <si>
+    <t>departed_mean</t>
+  </si>
+  <si>
+    <t>departed_sum</t>
+  </si>
+  <si>
+    <t>sum_diff</t>
+  </si>
+  <si>
+    <t>pct_diff</t>
+  </si>
+  <si>
+    <t>2/17/20</t>
+  </si>
+  <si>
+    <t>2/18/20</t>
+  </si>
+  <si>
+    <t>2/19/20</t>
+  </si>
+  <si>
+    <t>2/20/20</t>
+  </si>
+  <si>
+    <t>2/21/20</t>
+  </si>
+  <si>
+    <t>2/22/20</t>
+  </si>
+  <si>
+    <t>2/23/20</t>
+  </si>
+  <si>
+    <t>2/24/20</t>
+  </si>
+  <si>
+    <t>2/25/20</t>
+  </si>
+  <si>
+    <t>2/26/20</t>
+  </si>
+  <si>
+    <t>2/27/20</t>
+  </si>
+  <si>
+    <t>2/28/20</t>
+  </si>
+  <si>
+    <t>2/29/20</t>
+  </si>
+  <si>
+    <t>3/1/20</t>
+  </si>
+  <si>
+    <t>3/10/20</t>
+  </si>
+  <si>
+    <t>3/11/20</t>
+  </si>
+  <si>
+    <t>3/12/20</t>
+  </si>
+  <si>
+    <t>3/13/20</t>
+  </si>
+  <si>
+    <t>3/14/20</t>
+  </si>
+  <si>
+    <t>3/15/20</t>
+  </si>
+  <si>
+    <t>3/16/20</t>
+  </si>
+  <si>
+    <t>3/17/20</t>
+  </si>
+  <si>
+    <t>3/18/20</t>
+  </si>
+  <si>
+    <t>3/19/20</t>
+  </si>
+  <si>
+    <t>3/2/20</t>
+  </si>
+  <si>
+    <t>3/20/20</t>
+  </si>
+  <si>
+    <t>3/21/20</t>
+  </si>
+  <si>
+    <t>3/22/20</t>
+  </si>
+  <si>
+    <t>3/23/20</t>
+  </si>
+  <si>
+    <t>3/24/20</t>
+  </si>
+  <si>
+    <t>3/3/20</t>
+  </si>
+  <si>
+    <t>3/4/20</t>
+  </si>
+  <si>
+    <t>3/5/20</t>
+  </si>
+  <si>
+    <t>3/6/20</t>
+  </si>
+  <si>
+    <t>3/7/20</t>
+  </si>
+  <si>
+    <t>3/8/20</t>
+  </si>
+  <si>
+    <t>3/9/20</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,10 +186,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -57,14 +205,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -353,1037 +502,999 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date_</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>scheduled_mean</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>scheduled_sum</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>departed_mean</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>departed_sum</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>sum_diff</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>pct_diff</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2/17/20</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
         <v>618.5700000000001</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>17320</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>605.3200000000001</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>16949</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>-371</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>-2.19</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:8">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2/18/20</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
         <v>644.71</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>18052</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>625.6799999999999</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>17519</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>-533</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>-3.04</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2/19/20</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
         <v>638.89</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>17889</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>623.5</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>17458</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>-431</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>-2.47</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2/20/20</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
         <v>650.8200000000001</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>18223</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>632.9299999999999</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>17722</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>-501</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5">
         <v>-2.83</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2/21/20</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
         <v>656.61</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>18385</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>638.29</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>17872</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>-513</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>-2.87</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2/22/20</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
         <v>579.96</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>16239</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>568.96</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>15931</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>-308</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7">
         <v>-1.93</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:8">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2/23/20</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
         <v>583.96</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>16351</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>571.14</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>15992</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8">
         <v>-359</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8">
         <v>-2.24</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:8">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2/24/20</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
         <v>641.04</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>17949</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>625.36</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>17510</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>-439</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9">
         <v>-2.51</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:8">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2/25/20</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
         <v>642.6799999999999</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>17995</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>625.96</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>17527</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>-468</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10">
         <v>-2.67</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:8">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2/26/20</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
         <v>642.36</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>17986</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>620.11</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>17363</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11">
         <v>-623</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11">
         <v>-3.59</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:8">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2/27/20</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
         <v>660.14</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>18484</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>629.5700000000001</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12">
         <v>17628</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12">
         <v>-856</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12">
         <v>-4.86</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:8">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2/28/20</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
         <v>662.89</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13">
         <v>18561</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>641.14</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13">
         <v>17952</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13">
         <v>-609</v>
       </c>
-      <c r="H13" t="n">
+      <c r="H13">
         <v>-3.39</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:8">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>2/29/20</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
         <v>584.64</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14">
         <v>16370</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14">
         <v>568.11</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14">
         <v>15907</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14">
         <v>-463</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H14">
         <v>-2.91</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:8">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>3/1/20</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
         <v>585</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>16380</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15">
         <v>568.5</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15">
         <v>15918</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15">
         <v>-462</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H15">
         <v>-2.9</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:8">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>3/10/20</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
         <v>649.61</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16">
         <v>18189</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16">
         <v>629.54</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16">
         <v>17627</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16">
         <v>-562</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H16">
         <v>-3.19</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:8">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>3/11/20</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
         <v>651.89</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17">
         <v>18253</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17">
         <v>626.9299999999999</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F17">
         <v>17554</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G17">
         <v>-699</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H17">
         <v>-3.98</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:8">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>3/12/20</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
         <v>673.71</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18">
         <v>18864</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18">
         <v>650.86</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18">
         <v>18224</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G18">
         <v>-640</v>
       </c>
-      <c r="H18" t="n">
+      <c r="H18">
         <v>-3.51</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:8">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>3/13/20</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
         <v>678.04</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19">
         <v>18985</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19">
         <v>650.36</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19">
         <v>18210</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G19">
         <v>-775</v>
       </c>
-      <c r="H19" t="n">
+      <c r="H19">
         <v>-4.26</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:8">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>3/14/20</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
         <v>609.4299999999999</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20">
         <v>17064</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20">
         <v>585.4299999999999</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20">
         <v>16392</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20">
         <v>-672</v>
       </c>
-      <c r="H20" t="n">
+      <c r="H20">
         <v>-4.1</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:8">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>3/15/20</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
         <v>617.1799999999999</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21">
         <v>17281</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21">
         <v>588.36</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21">
         <v>16474</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G21">
         <v>-807</v>
       </c>
-      <c r="H21" t="n">
+      <c r="H21">
         <v>-4.9</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:8">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>3/16/20</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22">
         <v>658.46</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22">
         <v>18437</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22">
         <v>618.29</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F22">
         <v>17312</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G22">
         <v>-1125</v>
       </c>
-      <c r="H22" t="n">
+      <c r="H22">
         <v>-6.5</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:8">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>3/17/20</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23">
         <v>655.96</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23">
         <v>18367</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23">
         <v>601.11</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F23">
         <v>16831</v>
       </c>
-      <c r="G23" t="n">
+      <c r="G23">
         <v>-1536</v>
       </c>
-      <c r="H23" t="n">
+      <c r="H23">
         <v>-9.130000000000001</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:8">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>3/18/20</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24">
         <v>649.75</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24">
         <v>18193</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24">
         <v>565.6799999999999</v>
       </c>
-      <c r="F24" t="n">
+      <c r="F24">
         <v>15839</v>
       </c>
-      <c r="G24" t="n">
+      <c r="G24">
         <v>-2354</v>
       </c>
-      <c r="H24" t="n">
+      <c r="H24">
         <v>-14.86</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:8">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>3/19/20</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25">
         <v>664.4299999999999</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25">
         <v>18604</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25">
         <v>540.75</v>
       </c>
-      <c r="F25" t="n">
+      <c r="F25">
         <v>15141</v>
       </c>
-      <c r="G25" t="n">
+      <c r="G25">
         <v>-3463</v>
       </c>
-      <c r="H25" t="n">
+      <c r="H25">
         <v>-22.87</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:8">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>3/2/20</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26">
         <v>645.46</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26">
         <v>18073</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E26">
         <v>627.5700000000001</v>
       </c>
-      <c r="F26" t="n">
+      <c r="F26">
         <v>17572</v>
       </c>
-      <c r="G26" t="n">
+      <c r="G26">
         <v>-501</v>
       </c>
-      <c r="H26" t="n">
+      <c r="H26">
         <v>-2.85</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:8">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>3/20/20</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27">
         <v>665.39</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27">
         <v>18631</v>
       </c>
-      <c r="E27" t="n">
+      <c r="E27">
         <v>510.86</v>
       </c>
-      <c r="F27" t="n">
+      <c r="F27">
         <v>14304</v>
       </c>
-      <c r="G27" t="n">
+      <c r="G27">
         <v>-4327</v>
       </c>
-      <c r="H27" t="n">
+      <c r="H27">
         <v>-30.25</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
+    <row r="28" spans="1:8">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>3/21/20</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28">
         <v>605.39</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D28">
         <v>16951</v>
       </c>
-      <c r="E28" t="n">
+      <c r="E28">
         <v>440.82</v>
       </c>
-      <c r="F28" t="n">
+      <c r="F28">
         <v>12343</v>
       </c>
-      <c r="G28" t="n">
+      <c r="G28">
         <v>-4608</v>
       </c>
-      <c r="H28" t="n">
+      <c r="H28">
         <v>-37.33</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
+    <row r="29" spans="1:8">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>3/22/20</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29">
         <v>607.5</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D29">
         <v>17010</v>
       </c>
-      <c r="E29" t="n">
+      <c r="E29">
         <v>410.82</v>
       </c>
-      <c r="F29" t="n">
+      <c r="F29">
         <v>11503</v>
       </c>
-      <c r="G29" t="n">
+      <c r="G29">
         <v>-5507</v>
       </c>
-      <c r="H29" t="n">
+      <c r="H29">
         <v>-47.87</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
+    <row r="30" spans="1:8">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>3/3/20</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30">
+        <v>639.3200000000001</v>
+      </c>
+      <c r="D30">
+        <v>17901</v>
+      </c>
+      <c r="E30">
+        <v>381.61</v>
+      </c>
+      <c r="F30">
+        <v>10685</v>
+      </c>
+      <c r="G30">
+        <v>-7216</v>
+      </c>
+      <c r="H30">
+        <v>-67.53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31">
+        <v>637.3200000000001</v>
+      </c>
+      <c r="D31">
+        <v>17845</v>
+      </c>
+      <c r="E31">
+        <v>362.86</v>
+      </c>
+      <c r="F31">
+        <v>10160</v>
+      </c>
+      <c r="G31">
+        <v>-7685</v>
+      </c>
+      <c r="H31">
+        <v>-75.64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32">
         <v>643.75</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D32">
         <v>18025</v>
       </c>
-      <c r="E30" t="n">
+      <c r="E32">
         <v>625.36</v>
       </c>
-      <c r="F30" t="n">
+      <c r="F32">
         <v>17510</v>
       </c>
-      <c r="G30" t="n">
+      <c r="G32">
         <v>-515</v>
       </c>
-      <c r="H30" t="n">
+      <c r="H32">
         <v>-2.94</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>3/4/20</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
+    <row r="33" spans="1:8">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33">
         <v>644.5700000000001</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D33">
         <v>18048</v>
       </c>
-      <c r="E31" t="n">
+      <c r="E33">
         <v>626</v>
       </c>
-      <c r="F31" t="n">
+      <c r="F33">
         <v>17528</v>
       </c>
-      <c r="G31" t="n">
+      <c r="G33">
         <v>-520</v>
       </c>
-      <c r="H31" t="n">
+      <c r="H33">
         <v>-2.97</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>3/5/20</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
+    <row r="34" spans="1:8">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34">
         <v>681.86</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D34">
         <v>19092</v>
       </c>
-      <c r="E32" t="n">
+      <c r="E34">
         <v>644.11</v>
       </c>
-      <c r="F32" t="n">
+      <c r="F34">
         <v>18035</v>
       </c>
-      <c r="G32" t="n">
+      <c r="G34">
         <v>-1057</v>
       </c>
-      <c r="H32" t="n">
+      <c r="H34">
         <v>-5.86</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>3/6/20</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
+    <row r="35" spans="1:8">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35">
         <v>670.04</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D35">
         <v>18761</v>
       </c>
-      <c r="E33" t="n">
+      <c r="E35">
         <v>648.54</v>
       </c>
-      <c r="F33" t="n">
+      <c r="F35">
         <v>18159</v>
       </c>
-      <c r="G33" t="n">
+      <c r="G35">
         <v>-602</v>
       </c>
-      <c r="H33" t="n">
+      <c r="H35">
         <v>-3.32</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>3/7/20</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
+    <row r="36" spans="1:8">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36">
         <v>593.6799999999999</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D36">
         <v>16623</v>
       </c>
-      <c r="E34" t="n">
+      <c r="E36">
         <v>578.25</v>
       </c>
-      <c r="F34" t="n">
+      <c r="F36">
         <v>16191</v>
       </c>
-      <c r="G34" t="n">
+      <c r="G36">
         <v>-432</v>
       </c>
-      <c r="H34" t="n">
+      <c r="H36">
         <v>-2.67</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>3/8/20</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
+    <row r="37" spans="1:8">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37">
         <v>638.3200000000001</v>
       </c>
-      <c r="D35" t="n">
+      <c r="D37">
         <v>17873</v>
       </c>
-      <c r="E35" t="n">
+      <c r="E37">
         <v>620.5</v>
       </c>
-      <c r="F35" t="n">
+      <c r="F37">
         <v>17374</v>
       </c>
-      <c r="G35" t="n">
+      <c r="G37">
         <v>-499</v>
       </c>
-      <c r="H35" t="n">
+      <c r="H37">
         <v>-2.87</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>3/9/20</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
+    <row r="38" spans="1:8">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38">
         <v>648.89</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D38">
         <v>18169</v>
       </c>
-      <c r="E36" t="n">
+      <c r="E38">
         <v>631.21</v>
       </c>
-      <c r="F36" t="n">
+      <c r="F38">
         <v>17674</v>
       </c>
-      <c r="G36" t="n">
+      <c r="G38">
         <v>-495</v>
       </c>
-      <c r="H36" t="n">
+      <c r="H38">
         <v>-2.8</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>